<commit_message>
last videos + length from dowel when karman gaiting begins
</commit_message>
<xml_diff>
--- a/doweldist.xlsx
+++ b/doweldist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaans/Desktop/BIOL5380/FintasticBeasts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2980F355-0FCD-A24B-8FC5-CE16D5C99328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449E2943-3758-BC45-87DF-F27052D1AEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3800" yWindow="740" windowWidth="28040" windowHeight="17100" xr2:uid="{FB360ECC-1CA9-CB45-9A5D-66134185D57F}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="H9:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,29 +508,41 @@
       <c r="I16">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>35.58</v>
+      </c>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H17">
         <v>4</v>
       </c>
       <c r="I17">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>39.76</v>
+      </c>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H18">
         <v>5</v>
       </c>
       <c r="I18">
         <v>65</v>
       </c>
-    </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>37.54</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H19">
         <v>5</v>
       </c>
       <c r="I19">
         <v>85</v>
+      </c>
+      <c r="J19">
+        <v>54.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>